<commit_message>
Excel Test 3 Bongo Bongo
</commit_message>
<xml_diff>
--- a/assets/files/data/data_errors.xlsx
+++ b/assets/files/data/data_errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micha\WebstormProjects\electrondesktopjs\assets\files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D440B48-0E34-4941-B75B-39773D9FE52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF477F5-F805-46AB-9848-4E5E6283407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3B99372C-F313-4E6C-9D41-A964BEEC2E09}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8499" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8500" uniqueCount="207">
   <si>
     <t>Population</t>
   </si>
@@ -765,6 +765,9 @@
   <si>
     <t>bachelor</t>
   </si>
+  <si>
+    <t>Bongo Bongo</t>
+  </si>
 </sst>
 </file>
 
@@ -1216,9 +1219,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:EA167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BE87" sqref="BE87"/>
+      <selection pane="topRight" activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1257,9 @@
     <col min="58" max="58" width="25.7109375" customWidth="1"/>
     <col min="61" max="61" width="12.28515625" customWidth="1"/>
     <col min="62" max="62" width="16.7109375" customWidth="1"/>
+    <col min="67" max="67" width="8.85546875" customWidth="1"/>
+    <col min="68" max="68" width="25.85546875" customWidth="1"/>
+    <col min="69" max="69" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
@@ -2677,6 +2683,9 @@
       </c>
       <c r="AP8" t="s">
         <v>73</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">

</xml_diff>